<commit_message>
fix in 03_Elderly_fall_detection application for #18
</commit_message>
<xml_diff>
--- a/03_Elderly_fall_detection/Elderly_fall_detection_cam/exe/tinyyolov2_cam/tinyyolov2_cam_summary.xlsx
+++ b/03_Elderly_fall_detection/Elderly_fall_detection_cam/exe/tinyyolov2_cam/tinyyolov2_cam_summary.xlsx
@@ -900,7 +900,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>input.4</t>
+          <t>/module_list.0/conv_0/Conv_output_0</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -960,7 +960,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>input.8</t>
+          <t>/module_list.1/maxpool_1/MaxPool_output_0</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1020,7 +1020,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>input.16</t>
+          <t>/module_list.2/conv_2/Conv_output_0</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1080,7 +1080,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>input.20</t>
+          <t>/module_list.3/maxpool_3/MaxPool_output_0</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1140,7 +1140,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>input.28</t>
+          <t>/module_list.4/conv_4/Conv_output_0</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1200,7 +1200,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>input.32</t>
+          <t>/module_list.5/maxpool_5/MaxPool_output_0</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1260,7 +1260,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>input.40</t>
+          <t>/module_list.6/conv_6/Conv_output_0</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1320,7 +1320,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>input.44</t>
+          <t>/module_list.7/maxpool_7/MaxPool_output_0</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1380,7 +1380,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>input.52</t>
+          <t>/module_list.8/conv_8/Conv_output_0</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1440,7 +1440,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>input.56</t>
+          <t>/module_list.9/maxpool_9/MaxPool_output_0</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1500,7 +1500,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>input.64</t>
+          <t>/module_list.10/conv_10/Conv_output_0</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1560,7 +1560,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>input.68</t>
+          <t>/module_list.11/maxpool_11/MaxPool_output_0</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1620,7 +1620,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>input.76</t>
+          <t>/module_list.12/conv_12/Conv_output_0</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1680,7 +1680,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>input.88</t>
+          <t>/module_list.13/conv_13/Conv_output_0</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1782,7 +1782,7 @@
         <v>13</v>
       </c>
       <c r="O22" t="n">
-        <v>125</v>
+        <v>30</v>
       </c>
       <c r="P22" t="n">
         <v>13</v>
@@ -1791,7 +1791,7 @@
         <v>13</v>
       </c>
       <c r="S22" t="n">
-        <v>136</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23" outlineLevel="1">
@@ -1830,7 +1830,7 @@
         <v>0</v>
       </c>
       <c r="L23" t="n">
-        <v>125</v>
+        <v>30</v>
       </c>
       <c r="M23" t="n">
         <v>13</v>
@@ -1839,7 +1839,7 @@
         <v>13</v>
       </c>
       <c r="O23" t="n">
-        <v>125</v>
+        <v>30</v>
       </c>
       <c r="P23" t="n">
         <v>13</v>
@@ -1848,7 +1848,7 @@
         <v>13</v>
       </c>
       <c r="S23" t="n">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" outlineLevel="1">
@@ -1887,7 +1887,7 @@
         <v>0</v>
       </c>
       <c r="L24" t="n">
-        <v>125</v>
+        <v>30</v>
       </c>
       <c r="M24" t="n">
         <v>13</v>
@@ -1896,7 +1896,7 @@
         <v>13</v>
       </c>
       <c r="O24" t="n">
-        <v>125</v>
+        <v>30</v>
       </c>
       <c r="P24" t="n">
         <v>13</v>
@@ -1905,7 +1905,7 @@
         <v>13</v>
       </c>
       <c r="S24" t="n">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" outlineLevel="1">
@@ -1918,7 +1918,7 @@
         </is>
       </c>
       <c r="S25" t="n">
-        <v>33846</v>
+        <v>33808</v>
       </c>
     </row>
     <row r="26">

</xml_diff>